<commit_message>
replaced file with stephanie's fixed file
</commit_message>
<xml_diff>
--- a/week-2/Solutions/2-4-B-modeling-scenarios-solutions.xlsx
+++ b/week-2/Solutions/2-4-B-modeling-scenarios-solutions.xlsx
@@ -1,33 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10510"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\data-analytics-lectures\week-2\Solutions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sjones/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F590BA50-B56B-4E10-98C2-969797FDF5D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1DF6935-17EA-3641-B23A-661B38765893}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="18240" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1540" yWindow="2260" windowWidth="22020" windowHeight="14100" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Start" sheetId="2" state="hidden" r:id="rId1"/>
-    <sheet name="data-table-solutions" sheetId="3" r:id="rId2"/>
-    <sheet name="staffing-model-format" sheetId="4" r:id="rId3"/>
-    <sheet name="staffing-model-calc" sheetId="5" r:id="rId4"/>
+    <sheet name="warm-up" sheetId="6" r:id="rId2"/>
+    <sheet name="data-table-solutions" sheetId="3" r:id="rId3"/>
+    <sheet name="staffing-model-format" sheetId="4" r:id="rId4"/>
+    <sheet name="staffing-model-calc" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="CostItemSold" localSheetId="1">'data-table-solutions'!$B$3</definedName>
+    <definedName name="CostItemSold" localSheetId="2">'data-table-solutions'!$B$3</definedName>
+    <definedName name="CostItemSold" localSheetId="1">'warm-up'!$B$3</definedName>
     <definedName name="CostItemSold">Start!$B$2</definedName>
-    <definedName name="PostageCost" localSheetId="1">'data-table-solutions'!$B$2</definedName>
+    <definedName name="PostageCost" localSheetId="2">'data-table-solutions'!$B$2</definedName>
+    <definedName name="PostageCost" localSheetId="1">'warm-up'!$B$2</definedName>
     <definedName name="PostageCost">Start!$B$3</definedName>
-    <definedName name="SalesPrice" localSheetId="1">'data-table-solutions'!$B$1</definedName>
+    <definedName name="SalesPrice" localSheetId="2">'data-table-solutions'!$B$1</definedName>
+    <definedName name="SalesPrice" localSheetId="1">'warm-up'!$B$1</definedName>
     <definedName name="SalesPrice">Start!$B$1</definedName>
+    <definedName name="TotalProfit" localSheetId="1">'warm-up'!$B$15</definedName>
     <definedName name="TotalProfit">'data-table-solutions'!$B$15</definedName>
   </definedNames>
-  <calcPr calcId="191029" calcMode="autoNoTable"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +40,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -43,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="41">
   <si>
     <t>Total sales</t>
   </si>
@@ -183,18 +190,37 @@
   <si>
     <t>Above formulas</t>
   </si>
+  <si>
+    <t>Revenue per item</t>
+  </si>
+  <si>
+    <t>Cost of item</t>
+  </si>
+  <si>
+    <t>Shipping</t>
+  </si>
+  <si>
+    <t>Handling</t>
+  </si>
+  <si>
+    <t>Cost per item</t>
+  </si>
+  <si>
+    <t>Profit per item</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -242,7 +268,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -252,6 +278,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -322,7 +360,7 @@
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -363,19 +401,34 @@
     <xf numFmtId="5" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="8" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -666,12 +719,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -679,7 +732,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -687,7 +740,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -695,7 +748,7 @@
         <v>2.4900000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -704,7 +757,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -713,7 +766,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
@@ -722,7 +775,7 @@
         <v>2.4900000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -730,7 +783,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -738,7 +791,7 @@
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -746,7 +799,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
         <v>5</v>
       </c>
@@ -755,7 +808,7 @@
         <v>2.677</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
         <v>6</v>
       </c>
@@ -770,18 +823,439 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B3A6A9E-895C-C943-A675-A12D77153012}">
+  <dimension ref="A1:N17"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="35.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="32">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="F2" s="32">
+        <f>SalesPrice-(CostItemSold+B4+B5)</f>
+        <v>-0.6800000000000006</v>
+      </c>
+      <c r="G2">
+        <v>5</v>
+      </c>
+      <c r="H2">
+        <v>10</v>
+      </c>
+      <c r="I2">
+        <v>15</v>
+      </c>
+      <c r="J2">
+        <v>20</v>
+      </c>
+      <c r="K2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="32">
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+      <c r="G3">
+        <f t="dataTable" ref="G3:K7" dt2D="1" dtr="1" r1="B1" r2="B4"/>
+        <v>-0.6800000000000006</v>
+      </c>
+      <c r="H3">
+        <v>4.3199999999999994</v>
+      </c>
+      <c r="I3">
+        <v>9.32</v>
+      </c>
+      <c r="J3">
+        <v>14.32</v>
+      </c>
+      <c r="K3">
+        <v>19.32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="32">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>6</v>
+      </c>
+      <c r="G4">
+        <v>-3.6799999999999997</v>
+      </c>
+      <c r="H4">
+        <v>1.3200000000000003</v>
+      </c>
+      <c r="I4">
+        <v>6.32</v>
+      </c>
+      <c r="J4">
+        <v>11.32</v>
+      </c>
+      <c r="K4">
+        <v>16.32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="32">
+        <v>0.19</v>
+      </c>
+      <c r="F5">
+        <v>9</v>
+      </c>
+      <c r="G5">
+        <v>-6.68</v>
+      </c>
+      <c r="H5">
+        <v>-1.6799999999999997</v>
+      </c>
+      <c r="I5">
+        <v>3.3200000000000003</v>
+      </c>
+      <c r="J5">
+        <v>8.32</v>
+      </c>
+      <c r="K5">
+        <v>13.32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="33">
+        <v>5.68</v>
+      </c>
+      <c r="F6">
+        <v>12</v>
+      </c>
+      <c r="G6">
+        <v>-9.68</v>
+      </c>
+      <c r="H6">
+        <v>-4.68</v>
+      </c>
+      <c r="I6">
+        <v>0.32000000000000028</v>
+      </c>
+      <c r="J6">
+        <v>5.32</v>
+      </c>
+      <c r="K6">
+        <v>10.32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="F7">
+        <v>15</v>
+      </c>
+      <c r="G7">
+        <v>-12.680000000000003</v>
+      </c>
+      <c r="H7">
+        <v>-7.6800000000000033</v>
+      </c>
+      <c r="I7">
+        <v>-2.6800000000000033</v>
+      </c>
+      <c r="J7">
+        <v>2.3199999999999967</v>
+      </c>
+      <c r="K7">
+        <v>7.3199999999999967</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="33">
+        <v>-0.68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" s="32">
+        <f>SalesPrice-(CostItemSold+B4+B5)</f>
+        <v>-0.6800000000000006</v>
+      </c>
+      <c r="B12">
+        <v>5</v>
+      </c>
+      <c r="C12">
+        <v>10</v>
+      </c>
+      <c r="D12">
+        <v>15</v>
+      </c>
+      <c r="E12">
+        <v>20</v>
+      </c>
+      <c r="F12">
+        <v>25</v>
+      </c>
+      <c r="I12" s="34"/>
+      <c r="J12" s="34">
+        <v>5</v>
+      </c>
+      <c r="K12" s="34">
+        <v>10</v>
+      </c>
+      <c r="L12" s="34">
+        <v>15</v>
+      </c>
+      <c r="M12" s="34">
+        <v>20</v>
+      </c>
+      <c r="N12" s="34">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13">
+        <f t="dataTable" ref="B13:F17" dt2D="1" dtr="1" r1="B1" r2="B4" ca="1"/>
+        <v>-0.6800000000000006</v>
+      </c>
+      <c r="C13">
+        <v>4.3199999999999994</v>
+      </c>
+      <c r="D13">
+        <v>9.32</v>
+      </c>
+      <c r="E13">
+        <v>14.32</v>
+      </c>
+      <c r="F13">
+        <v>19.32</v>
+      </c>
+      <c r="I13" s="34">
+        <v>3</v>
+      </c>
+      <c r="J13" s="34">
+        <v>-0.6800000000000006</v>
+      </c>
+      <c r="K13" s="34">
+        <v>4.3199999999999994</v>
+      </c>
+      <c r="L13" s="34">
+        <v>9.32</v>
+      </c>
+      <c r="M13" s="34">
+        <v>14.32</v>
+      </c>
+      <c r="N13" s="34">
+        <v>19.32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14">
+        <v>6</v>
+      </c>
+      <c r="B14">
+        <v>-3.6799999999999997</v>
+      </c>
+      <c r="C14">
+        <v>1.3200000000000003</v>
+      </c>
+      <c r="D14">
+        <v>6.32</v>
+      </c>
+      <c r="E14">
+        <v>11.32</v>
+      </c>
+      <c r="F14">
+        <v>16.32</v>
+      </c>
+      <c r="I14" s="34">
+        <v>6</v>
+      </c>
+      <c r="J14" s="34">
+        <v>-3.6799999999999997</v>
+      </c>
+      <c r="K14" s="34">
+        <v>1.3200000000000003</v>
+      </c>
+      <c r="L14" s="34">
+        <v>6.32</v>
+      </c>
+      <c r="M14" s="34">
+        <v>11.32</v>
+      </c>
+      <c r="N14" s="34">
+        <v>16.32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15">
+        <v>9</v>
+      </c>
+      <c r="B15">
+        <v>-6.68</v>
+      </c>
+      <c r="C15">
+        <v>-1.6799999999999997</v>
+      </c>
+      <c r="D15">
+        <v>3.3200000000000003</v>
+      </c>
+      <c r="E15">
+        <v>8.32</v>
+      </c>
+      <c r="F15">
+        <v>13.32</v>
+      </c>
+      <c r="I15" s="34">
+        <v>9</v>
+      </c>
+      <c r="J15" s="34">
+        <v>-6.68</v>
+      </c>
+      <c r="K15" s="34">
+        <v>-1.6799999999999997</v>
+      </c>
+      <c r="L15" s="34">
+        <v>3.3200000000000003</v>
+      </c>
+      <c r="M15" s="34">
+        <v>8.32</v>
+      </c>
+      <c r="N15" s="34">
+        <v>13.32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16">
+        <v>12</v>
+      </c>
+      <c r="B16">
+        <v>-9.68</v>
+      </c>
+      <c r="C16">
+        <v>-4.68</v>
+      </c>
+      <c r="D16">
+        <v>0.32000000000000028</v>
+      </c>
+      <c r="E16">
+        <v>5.32</v>
+      </c>
+      <c r="F16">
+        <v>10.32</v>
+      </c>
+      <c r="I16" s="34">
+        <v>12</v>
+      </c>
+      <c r="J16" s="34">
+        <v>-9.68</v>
+      </c>
+      <c r="K16" s="34">
+        <v>-4.68</v>
+      </c>
+      <c r="L16" s="34">
+        <v>0.32000000000000028</v>
+      </c>
+      <c r="M16" s="34">
+        <v>5.32</v>
+      </c>
+      <c r="N16" s="34">
+        <v>10.32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>-12.680000000000003</v>
+      </c>
+      <c r="C17">
+        <v>-7.6800000000000033</v>
+      </c>
+      <c r="D17">
+        <v>-2.6800000000000033</v>
+      </c>
+      <c r="E17">
+        <v>2.3199999999999967</v>
+      </c>
+      <c r="F17">
+        <v>7.3199999999999967</v>
+      </c>
+      <c r="I17" s="34">
+        <v>15</v>
+      </c>
+      <c r="J17" s="34">
+        <v>-12.680000000000003</v>
+      </c>
+      <c r="K17" s="34">
+        <v>-7.6800000000000033</v>
+      </c>
+      <c r="L17" s="34">
+        <v>-2.6800000000000033</v>
+      </c>
+      <c r="M17" s="34">
+        <v>2.3199999999999967</v>
+      </c>
+      <c r="N17" s="34">
+        <v>7.3199999999999967</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B20:F24">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -789,7 +1263,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -797,7 +1271,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -805,7 +1279,7 @@
         <v>2.4900000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -818,7 +1292,7 @@
         <v>=SalesPrice</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -831,7 +1305,7 @@
         <v>=CostItemSold</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
@@ -844,7 +1318,7 @@
         <v>=PostageCost</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -852,7 +1326,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -860,7 +1334,7 @@
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -868,7 +1342,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
         <v>5</v>
       </c>
@@ -881,7 +1355,7 @@
         <v>=SUM(B9:B12)</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
         <v>6</v>
       </c>
@@ -894,12 +1368,12 @@
         <v>=B6-B13</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19">
         <f>TotalProfit</f>
         <v>1.8130000000000002</v>
@@ -920,7 +1394,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6">
       <c r="A20">
         <v>3</v>
       </c>
@@ -941,7 +1415,7 @@
         <v>21.812999999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6">
       <c r="A21">
         <v>6</v>
       </c>
@@ -961,7 +1435,7 @@
         <v>18.812999999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6">
       <c r="A22">
         <v>9</v>
       </c>
@@ -981,7 +1455,7 @@
         <v>15.813000000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6">
       <c r="A23">
         <v>12</v>
       </c>
@@ -1001,7 +1475,7 @@
         <v>12.813000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6">
       <c r="A24">
         <v>15</v>
       </c>
@@ -1031,32 +1505,32 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A19CF3B6-7AC3-4096-88CD-70F277EF0B53}">
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" customWidth="1"/>
+    <col min="1" max="1" width="30.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="16">
       <c r="A1" s="17" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="B2" s="7" t="s">
         <v>30</v>
       </c>
@@ -1070,7 +1544,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -1088,7 +1562,7 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -1106,7 +1580,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -1124,7 +1598,7 @@
         <v>7000000</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -1142,7 +1616,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -1160,7 +1634,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -1178,7 +1652,7 @@
         <v>125000</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="B10" s="7" t="s">
         <v>24</v>
       </c>
@@ -1195,8 +1669,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="10.9" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="11" customHeight="1"/>
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -1208,12 +1682,12 @@
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -1223,7 +1697,7 @@
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1233,7 +1707,7 @@
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1243,7 +1717,7 @@
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -1253,7 +1727,7 @@
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -1263,7 +1737,7 @@
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6">
       <c r="A20" s="1" t="s">
         <v>12</v>
       </c>
@@ -1278,47 +1752,47 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEBF9E46-8199-4A65-8DD9-C36562EEEB26}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" customWidth="1"/>
+    <col min="1" max="1" width="30.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C2" s="33" t="s">
+    <row r="2" spans="1:6">
+      <c r="C2" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="32" t="s">
+      <c r="D2" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="31" t="s">
+      <c r="E2" s="29" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="16">
+      <c r="B3" s="35">
         <f t="shared" ref="B3:B8" si="0">D3</f>
         <v>10000</v>
       </c>
@@ -1332,11 +1806,11 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="30">
+      <c r="B4" s="36">
         <f t="shared" si="0"/>
         <v>0.04</v>
       </c>
@@ -1350,29 +1824,29 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="37">
         <f t="shared" si="0"/>
         <v>8000000</v>
       </c>
       <c r="C5" s="8">
         <v>9000000</v>
       </c>
-      <c r="D5" s="29">
+      <c r="D5" s="28">
         <v>8000000</v>
       </c>
       <c r="E5" s="8">
         <v>7000000</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="28">
+      <c r="B6" s="38">
         <f t="shared" si="0"/>
         <v>0.03</v>
       </c>
@@ -1386,11 +1860,11 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="37">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
@@ -1404,11 +1878,11 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="37">
         <f t="shared" si="0"/>
         <v>150000</v>
       </c>
@@ -1422,7 +1896,7 @@
         <v>125000</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="B10" s="7" t="s">
         <v>24</v>
       </c>
@@ -1439,8 +1913,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="10.9" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="11" customHeight="1"/>
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -1464,7 +1938,7 @@
         <v>116985.85600000001</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -1489,7 +1963,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -1498,11 +1972,11 @@
         <v>20</v>
       </c>
       <c r="C14" s="9">
-        <f t="shared" ref="C14:F15" si="1">B14*(1+$B$6)</f>
+        <f>B14*(1+$B$6)</f>
         <v>20.6</v>
       </c>
       <c r="D14" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="D14:F15" si="1">C14*(1+$B$6)</f>
         <v>21.218000000000004</v>
       </c>
       <c r="E14" s="9">
@@ -1514,7 +1988,7 @@
         <v>22.510176200000004</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1523,7 +1997,7 @@
         <v>150000</v>
       </c>
       <c r="C15" s="25">
-        <f t="shared" si="1"/>
+        <f>B15*(1+$B$6)</f>
         <v>154500</v>
       </c>
       <c r="D15" s="25">
@@ -1539,7 +2013,7 @@
         <v>168826.32150000002</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1564,7 +2038,7 @@
         <v>9004070.4800000004</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -1589,7 +2063,7 @@
         <v>2633372.2314678282</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -1614,7 +2088,7 @@
         <v>2025915.8580000002</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6">
       <c r="A20" s="1" t="s">
         <v>12</v>
       </c>
@@ -1639,12 +2113,12 @@
         <v>13663358.56946783</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6">
       <c r="B22" s="24" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="32">
       <c r="A24" t="s">
         <v>19</v>
       </c>
@@ -1668,7 +2142,7 @@
         <v>=E12*(1+$B$4)</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="32">
       <c r="A25" t="s">
         <v>18</v>
       </c>
@@ -1693,7 +2167,7 @@
         <v>=ROUNDUP(F12/$B$3,0)</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="32">
       <c r="A26" t="s">
         <v>17</v>
       </c>
@@ -1718,7 +2192,7 @@
         <v>=E14*(1+$B$6)</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="32">
       <c r="A27" t="s">
         <v>16</v>
       </c>
@@ -1743,14 +2217,14 @@
         <v>=E15*(1+$B$6)</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6">
       <c r="B28" s="19"/>
       <c r="C28" s="19"/>
       <c r="D28" s="19"/>
       <c r="E28" s="19"/>
       <c r="F28" s="19"/>
     </row>
-    <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="32">
       <c r="A29" t="s">
         <v>15</v>
       </c>
@@ -1775,7 +2249,7 @@
         <v>=E17*(1+$B$6)</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="16">
       <c r="A30" t="s">
         <v>14</v>
       </c>
@@ -1800,7 +2274,7 @@
         <v>=F12*F14</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="16">
       <c r="A31" t="s">
         <v>13</v>
       </c>
@@ -1825,7 +2299,7 @@
         <v>=F15*F13</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="32">
       <c r="A32" s="1" t="s">
         <v>12</v>
       </c>

</xml_diff>